<commit_message>
updating repo with Track_models.xlsx
</commit_message>
<xml_diff>
--- a/bitcoin_price_predictor/models/Track_models.xlsx
+++ b/bitcoin_price_predictor/models/Track_models.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedro/Desktop/BTCdata/models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedro/code/pedrojfsantos/bitcoin_price_predictor/bitcoin_price_predictor/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA93DC56-BE6A-DE4F-A435-2BCE943901DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F27CF4C-DD24-2848-AAB5-45803C127D07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{A9279D7E-5379-9A49-B076-060697C609E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Price Oil</t>
   </si>
@@ -81,20 +81,74 @@
     <t>RNN_base with BTC, USD, 2019 tweest features</t>
   </si>
   <si>
-    <t>vix index</t>
-  </si>
-  <si>
-    <t>S&amp;P500</t>
-  </si>
-  <si>
-    <t>Dow Jones</t>
+    <t>RNN_base with BTC/USD</t>
+  </si>
+  <si>
+    <t>BTC-USD</t>
+  </si>
+  <si>
+    <t>GOOG</t>
+  </si>
+  <si>
+    <t>GC=F</t>
+  </si>
+  <si>
+    <t>TSLA</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Round 1</t>
+  </si>
+  <si>
+    <t>Round 2</t>
+  </si>
+  <si>
+    <t>Round 3</t>
+  </si>
+  <si>
+    <t>Round 4</t>
+  </si>
+  <si>
+    <t>Round 5</t>
+  </si>
+  <si>
+    <t>Round 6</t>
+  </si>
+  <si>
+    <t>MEAN</t>
+  </si>
+  <si>
+    <t>RNN_base_PJS_23Nov2020</t>
+  </si>
+  <si>
+    <t>'NEM'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'NOG'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '^GSPC'</t>
+  </si>
+  <si>
+    <t>'MSFT'</t>
+  </si>
+  <si>
+    <t>'AAPL'</t>
+  </si>
+  <si>
+    <t>'^IXIC'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -126,8 +180,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Monaco"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,8 +232,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -209,11 +289,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -221,26 +330,66 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,72 +730,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43C85B9-8075-D44D-9B7A-FC3E727A44A3}">
-  <dimension ref="B1:L19"/>
+  <dimension ref="B1:O33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.1640625" customWidth="1"/>
-    <col min="3" max="12" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="C1" s="9" t="s">
+    <row r="1" spans="2:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-    </row>
-    <row r="2" spans="2:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="B2" s="3"/>
-      <c r="C2" s="7" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2" spans="2:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="B2" s="25"/>
+      <c r="C2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-    </row>
-    <row r="3" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="G2" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+    </row>
+    <row r="3" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="3">
         <v>0.53</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="3">
         <v>0.7</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="3">
         <v>0.3478</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="3">
         <v>0.47826000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="G3" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="1">
@@ -661,9 +821,15 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="1">
@@ -678,9 +844,15 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="28" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="1">
@@ -695,9 +867,15 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="28" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1">
@@ -712,9 +890,15 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1">
@@ -729,9 +913,15 @@
       <c r="F8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="2">
@@ -746,9 +936,15 @@
       <c r="F9" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="29" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="1">
@@ -763,9 +959,15 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="29" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="1">
@@ -780,9 +982,15 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="2">
@@ -797,9 +1005,16 @@
       <c r="F12" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="N12" s="20"/>
+    </row>
+    <row r="13" spans="2:15" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="2">
@@ -814,9 +1029,15 @@
       <c r="F13" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="29" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="2">
@@ -831,9 +1052,16 @@
       <c r="F14" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="O14" s="20"/>
+    </row>
+    <row r="15" spans="2:15" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="29" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="2">
@@ -848,27 +1076,385 @@
       <c r="F15" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="B17" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="B18" s="4" t="s">
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="29" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="B19" s="4" t="s">
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="21">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="29" t="s">
         <v>20</v>
       </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="21">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="21">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="21">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="21">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="21">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" s="21">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="21">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="21">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="21">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+    </row>
+    <row r="27" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B27" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="13">
+        <v>0.59419999999999995</v>
+      </c>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+    </row>
+    <row r="28" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B28" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+    </row>
+    <row r="29" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="14">
+        <v>0.59419999999999995</v>
+      </c>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+    </row>
+    <row r="30" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B30" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="15">
+        <v>0.39855000000000002</v>
+      </c>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+    </row>
+    <row r="31" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B31" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="15">
+        <v>0.57969999999999999</v>
+      </c>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+    </row>
+    <row r="32" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B32" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="16">
+        <v>0.59519999999999995</v>
+      </c>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+    </row>
+    <row r="33" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="B33" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="19">
+        <f>AVERAGE(H27:H32)</f>
+        <v>0.54364166666666669</v>
+      </c>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C1:L1"/>
+  <mergeCells count="2">
+    <mergeCell ref="B26:L26"/>
+    <mergeCell ref="B1:L1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C4:F15">
+  <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="C4:H25">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>